<commit_message>
Android Ready number 1
</commit_message>
<xml_diff>
--- a/document/Keys.xlsx
+++ b/document/Keys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\ardenne\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA19DBED-730D-4FC3-A277-AB7BC9188C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944325F8-8DDA-4C0B-A3C4-240A418A0A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6492" yWindow="6492" windowWidth="34560" windowHeight="18684" xr2:uid="{A84F5C5C-25E3-49E2-B607-EEA0F203E0F6}"/>
+    <workbookView xWindow="7608" yWindow="2652" windowWidth="13128" windowHeight="18684" xr2:uid="{A84F5C5C-25E3-49E2-B607-EEA0F203E0F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="239">
   <si>
     <t>JF8DA-BA82G-WZ6J6</t>
   </si>
@@ -640,16 +640,142 @@
   </si>
   <si>
     <t>Email Address</t>
+  </si>
+  <si>
+    <t>Steve Komor</t>
+  </si>
+  <si>
+    <t>plpba  pat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jerry Hagler </t>
+  </si>
+  <si>
+    <t>Erich Swaford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Franco Madiera </t>
+  </si>
+  <si>
+    <t>Cristopher Henry</t>
+  </si>
+  <si>
+    <t>Casey</t>
+  </si>
+  <si>
+    <t>vladislav</t>
+  </si>
+  <si>
+    <t>JustSabien</t>
+  </si>
+  <si>
+    <t>Grandma</t>
+  </si>
+  <si>
+    <t>Game Club</t>
+  </si>
+  <si>
+    <t>Amana Peet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mich I Reiter </t>
+  </si>
+  <si>
+    <t>Edward bawerman</t>
+  </si>
+  <si>
+    <t>PCGamer</t>
+  </si>
+  <si>
+    <t>Tran Toai</t>
+  </si>
+  <si>
+    <t>Maarnuwel</t>
+  </si>
+  <si>
+    <t>kotaku</t>
+  </si>
+  <si>
+    <t>rich@pcgames</t>
+  </si>
+  <si>
+    <t>cameron</t>
+  </si>
+  <si>
+    <t>RockPaperShotgun</t>
+  </si>
+  <si>
+    <t>Joe and Jack</t>
+  </si>
+  <si>
+    <t>Nuno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boardgame Chronicle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pixelated </t>
+  </si>
+  <si>
+    <t>saveorquit</t>
+  </si>
+  <si>
+    <t>deadpixels</t>
+  </si>
+  <si>
+    <t>indiemag</t>
+  </si>
+  <si>
+    <t>phongbientap</t>
+  </si>
+  <si>
+    <t>felix</t>
+  </si>
+  <si>
+    <t>Sanjar</t>
+  </si>
+  <si>
+    <t>Luke wilson</t>
+  </si>
+  <si>
+    <t>Xia0</t>
+  </si>
+  <si>
+    <t>Karl</t>
+  </si>
+  <si>
+    <t>Emote</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Lance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -672,13 +798,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -993,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8218D775-FB64-4BF3-BDD6-7A776E902564}">
   <dimension ref="A1:C200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1019,313 +1151,481 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="21" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="21" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -2011,6 +2311,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B31" r:id="rId1" xr:uid="{6E6A9C87-68AD-48D7-ACB6-CEACAAB06B79}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix Bug loading Supply game
</commit_message>
<xml_diff>
--- a/document/Keys.xlsx
+++ b/document/Keys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\ardenne\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424903B0-F4C1-4A54-B92B-757950649922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F970C3-FCE2-4569-989D-21E5CAB412C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7608" yWindow="2652" windowWidth="13128" windowHeight="18684" xr2:uid="{A84F5C5C-25E3-49E2-B607-EEA0F203E0F6}"/>
+    <workbookView xWindow="25008" yWindow="4212" windowWidth="13128" windowHeight="18684" xr2:uid="{A84F5C5C-25E3-49E2-B607-EEA0F203E0F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="241">
   <si>
     <t>JF8DA-BA82G-WZ6J6</t>
   </si>
@@ -754,6 +754,9 @@
   </si>
   <si>
     <t>Gold Bear</t>
+  </si>
+  <si>
+    <t>Damon</t>
   </si>
 </sst>
 </file>
@@ -1128,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8218D775-FB64-4BF3-BDD6-7A776E902564}">
   <dimension ref="A1:C200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1610,15 +1613,24 @@
       <c r="A59" t="s">
         <v>58</v>
       </c>
+      <c r="B59" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
+      <c r="B60" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>